<commit_message>
Git batch file commit
</commit_message>
<xml_diff>
--- a/QAFox/src/test/resources/testdata/testData.xlsx
+++ b/QAFox/src/test/resources/testdata/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT_All_Local_Repo\GIT_Local_QAFox_Automation\QAFox\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9D62F7-6179-4556-82EC-E1A069AA74C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B24372-0077-42DB-85D1-D5831424446D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,7 +121,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -473,7 +473,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -499,6 +499,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{135EAEE0-414C-44A3-BE91-DF6BD4AC1C51}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{E83F0A72-FA97-48F4-B547-F82C4FB5C588}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Git batch file commit June 03
</commit_message>
<xml_diff>
--- a/QAFox/src/test/resources/testdata/testData.xlsx
+++ b/QAFox/src/test/resources/testdata/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT_All_Local_Repo\GIT_Local_QAFox_Automation\QAFox\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD4B20D-8760-4CFF-B230-D520B2804A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BE7133-D2BE-4A04-89DB-4DF0DE946E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
     <t>Automation@123</t>
   </si>
   <si>
-    <t>selenium3888223</t>
+    <t>newUser34422</t>
   </si>
 </sst>
 </file>
@@ -429,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -443,7 +443,7 @@
     <col min="6" max="6" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.7265625" customWidth="1"/>
     <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.54296875" bestFit="1" customWidth="1"/>
   </cols>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0206869-1BA9-4A13-8B52-ED6024235FE4}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>